<commit_message>
Updating Forms for 2018 Round - LocationDetails   - Remove INE questions on Location Details - DONE! - IndividualDetails   - Update relevent condition of questions (26.fatherAlive, 27.motherAlive) to ${age}<18 - DONE!   - Add condition age>=18 to questions 24.7.hasDrivingLicense and 24.8.hasVoterCard   - Updated education options - Add new questions (31.1 -> 32.2)
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/in_migration.xlsx
+++ b/xforms/xlsforms/in_migration.xlsx
@@ -859,10 +859,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -900,14 +900,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -915,18 +907,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -947,6 +932,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -954,16 +946,29 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -978,45 +983,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1036,7 +1004,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1044,6 +1019,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1108,7 +1108,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1120,55 +1234,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1180,31 +1258,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1216,67 +1276,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1330,32 +1330,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1387,151 +1361,177 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2020,11 +2020,11 @@
   <dimension ref="A1:R93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M31" sqref="M31"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88" defaultRowHeight="12"/>
@@ -3026,8 +3026,8 @@
   <sheetPr/>
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65:E66"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88" defaultRowHeight="12" outlineLevelCol="4"/>

</xml_diff>

<commit_message>
- Add "0. O proprio chefe" in relationship with head of origin and destiny - Add option "Deficiente Visual" for the question canTestReading in individual details form
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/in_migration.xlsx
+++ b/xforms/xlsforms/in_migration.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13125" tabRatio="500"/>
+    <workbookView windowWidth="20385" windowHeight="8430" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267">
   <si>
     <t>type</t>
   </si>
@@ -723,6 +723,9 @@
   </si>
   <si>
     <t>relation_with_head</t>
+  </si>
+  <si>
+    <t>O Proprio chefe</t>
   </si>
   <si>
     <t>Pai/Mãe</t>
@@ -859,9 +862,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
@@ -900,26 +903,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -932,12 +927,72 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -954,31 +1009,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -997,39 +1030,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1102,7 +1105,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1114,85 +1243,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1204,79 +1279,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1287,30 +1290,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1325,39 +1304,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1387,151 +1333,208 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1543,10 +1546,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2019,8 +2022,8 @@
   <sheetPr/>
   <dimension ref="A1:R93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -2163,20 +2166,20 @@
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
     </row>
-    <row r="5" s="4" customFormat="1" ht="15" customHeight="1" spans="1:16">
+    <row r="5" s="3" customFormat="1" ht="15" customHeight="1" spans="1:16">
       <c r="A5" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>24</v>
       </c>
       <c r="F5" s="22"/>
@@ -2195,20 +2198,20 @@
       <c r="O5" s="22"/>
       <c r="P5" s="22"/>
     </row>
-    <row r="6" s="4" customFormat="1" ht="15" customHeight="1" spans="1:16">
+    <row r="6" s="3" customFormat="1" ht="15" customHeight="1" spans="1:16">
       <c r="A6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>27</v>
       </c>
       <c r="F6" s="22"/>
@@ -2657,7 +2660,7 @@
       <c r="B26" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>109</v>
       </c>
       <c r="D26" s="37" t="s">
@@ -2669,7 +2672,7 @@
       <c r="J26" s="31" t="b">
         <v>1</v>
       </c>
-      <c r="M26" s="4" t="s">
+      <c r="M26" s="3" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2751,7 +2754,7 @@
       <c r="B30" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>125</v>
       </c>
       <c r="D30" s="19" t="s">
@@ -2763,7 +2766,7 @@
       <c r="J30" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="M30" s="4" t="s">
+      <c r="M30" s="3" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2800,7 +2803,7 @@
       <c r="B32" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>133</v>
       </c>
       <c r="D32" s="19" t="s">
@@ -2839,26 +2842,26 @@
         <v>137</v>
       </c>
     </row>
-    <row r="34" s="4" customFormat="1" spans="1:13">
-      <c r="A34" s="4" t="s">
+    <row r="34" s="3" customFormat="1" spans="1:13">
+      <c r="A34" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="3" t="s">
         <v>140</v>
       </c>
       <c r="J34" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="M34" s="4" t="s">
+      <c r="M34" s="3" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3024,10 +3027,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A31" sqref="$A31:$XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88" defaultRowHeight="12" outlineLevelCol="4"/>
@@ -3548,20 +3551,20 @@
         <v>221</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="8" t="s">
+    <row r="31" s="3" customFormat="1" spans="1:5">
+      <c r="A31" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="B31" s="9">
-        <v>1</v>
-      </c>
-      <c r="C31" s="10" t="s">
+      <c r="B31" s="11">
+        <v>0</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="12" t="s">
         <v>223</v>
       </c>
     </row>
@@ -3570,7 +3573,7 @@
         <v>222</v>
       </c>
       <c r="B32" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>224</v>
@@ -3587,7 +3590,7 @@
         <v>222</v>
       </c>
       <c r="B33" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>225</v>
@@ -3604,7 +3607,7 @@
         <v>222</v>
       </c>
       <c r="B34" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>226</v>
@@ -3621,7 +3624,7 @@
         <v>222</v>
       </c>
       <c r="B35" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>227</v>
@@ -3638,7 +3641,7 @@
         <v>222</v>
       </c>
       <c r="B36" s="9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>228</v>
@@ -3655,7 +3658,7 @@
         <v>222</v>
       </c>
       <c r="B37" s="9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>229</v>
@@ -3672,7 +3675,7 @@
         <v>222</v>
       </c>
       <c r="B38" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C38" s="10" t="s">
         <v>230</v>
@@ -3689,7 +3692,7 @@
         <v>222</v>
       </c>
       <c r="B39" s="9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>231</v>
@@ -3706,7 +3709,7 @@
         <v>222</v>
       </c>
       <c r="B40" s="9">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>232</v>
@@ -3723,7 +3726,7 @@
         <v>222</v>
       </c>
       <c r="B41" s="9">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>233</v>
@@ -3740,7 +3743,7 @@
         <v>222</v>
       </c>
       <c r="B42" s="9">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>234</v>
@@ -3757,7 +3760,7 @@
         <v>222</v>
       </c>
       <c r="B43" s="9">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>235</v>
@@ -3773,59 +3776,59 @@
       <c r="A44" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="B44" s="11">
-        <v>98</v>
+      <c r="B44" s="9">
+        <v>13</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>187</v>
+        <v>236</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>187</v>
+        <v>236</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>187</v>
+        <v>236</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="B45" s="9">
+      <c r="B45" s="11">
+        <v>98</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B46" s="9">
         <v>88</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C46" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D46" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E46" s="10" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="46" s="3" customFormat="1" spans="1:5">
-      <c r="A46" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="B46" s="9">
-        <v>1</v>
-      </c>
-      <c r="C46" s="10" t="s">
+    <row r="47" s="4" customFormat="1" spans="1:5">
+      <c r="A47" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="D46" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="3" t="s">
-        <v>236</v>
-      </c>
       <c r="B47" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C47" s="10" t="s">
         <v>238</v>
@@ -3838,11 +3841,11 @@
       </c>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="3" t="s">
-        <v>236</v>
+      <c r="A48" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="B48" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>239</v>
@@ -3855,31 +3858,31 @@
       </c>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="3" t="s">
-        <v>236</v>
+      <c r="A49" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="B49" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>240</v>
       </c>
       <c r="D49" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B50" s="9">
+        <v>4</v>
+      </c>
+      <c r="C50" s="10" t="s">
         <v>241</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="B50" s="9">
-        <v>5</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>242</v>
       </c>
       <c r="D50" s="10" t="s">
         <v>242</v>
@@ -3889,11 +3892,11 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="3" t="s">
-        <v>236</v>
+      <c r="A51" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="B51" s="9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>243</v>
@@ -3906,11 +3909,11 @@
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="3" t="s">
-        <v>236</v>
+      <c r="A52" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="B52" s="9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>244</v>
@@ -3923,11 +3926,11 @@
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="3" t="s">
-        <v>236</v>
+      <c r="A53" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="B53" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C53" s="10" t="s">
         <v>245</v>
@@ -3940,11 +3943,11 @@
       </c>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="3" t="s">
-        <v>236</v>
+      <c r="A54" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="B54" s="9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C54" s="10" t="s">
         <v>246</v>
@@ -3957,11 +3960,11 @@
       </c>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="3" t="s">
-        <v>236</v>
+      <c r="A55" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="B55" s="9">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C55" s="10" t="s">
         <v>247</v>
@@ -3974,11 +3977,11 @@
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="3" t="s">
-        <v>236</v>
+      <c r="A56" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="B56" s="9">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C56" s="10" t="s">
         <v>248</v>
@@ -3991,11 +3994,11 @@
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="3" t="s">
-        <v>236</v>
+      <c r="A57" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="B57" s="9">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>249</v>
@@ -4008,11 +4011,11 @@
       </c>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="3" t="s">
-        <v>236</v>
+      <c r="A58" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="B58" s="9">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>250</v>
@@ -4025,11 +4028,11 @@
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="3" t="s">
-        <v>236</v>
+      <c r="A59" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="B59" s="9">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>251</v>
@@ -4042,11 +4045,11 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="3" t="s">
-        <v>236</v>
+      <c r="A60" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="B60" s="9">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C60" s="10" t="s">
         <v>252</v>
@@ -4059,11 +4062,11 @@
       </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="3" t="s">
-        <v>236</v>
+      <c r="A61" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="B61" s="9">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C61" s="10" t="s">
         <v>253</v>
@@ -4076,11 +4079,11 @@
       </c>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="3" t="s">
-        <v>236</v>
+      <c r="A62" s="4" t="s">
+        <v>237</v>
       </c>
       <c r="B62" s="9">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C62" s="10" t="s">
         <v>254</v>
@@ -4093,107 +4096,124 @@
       </c>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="B63" s="11">
+      <c r="A63" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B63" s="9">
+        <v>17</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B64" s="11">
         <v>98</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C64" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="D63" s="10" t="s">
+      <c r="D64" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="E63" s="10" t="s">
+      <c r="E64" s="10" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="B64" s="9">
+    <row r="65" spans="1:5">
+      <c r="A65" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B65" s="9">
         <v>88</v>
       </c>
-      <c r="C64" s="10" t="s">
+      <c r="C65" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="D64" s="10" t="s">
+      <c r="D65" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="E64" s="10" t="s">
+      <c r="E65" s="10" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="65" s="4" customFormat="1" spans="1:5">
-      <c r="A65" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="B65" s="17">
-        <v>1</v>
-      </c>
-      <c r="C65" s="4" t="s">
+    <row r="66" s="3" customFormat="1" spans="1:5">
+      <c r="A66" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="B66" s="17">
+        <v>1</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="67" s="3" customFormat="1" spans="1:5">
+      <c r="A67" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="E65" s="4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="66" s="4" customFormat="1" spans="1:5">
-      <c r="A66" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="B66" s="11">
+      <c r="B67" s="11">
         <v>2</v>
       </c>
-      <c r="C66" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="D66" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="E66" s="12" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="3"/>
-      <c r="B67" s="9"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
+      <c r="C67" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="E67" s="12" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="3"/>
+      <c r="A68" s="4"/>
       <c r="B68" s="9"/>
       <c r="C68" s="10"/>
       <c r="D68" s="10"/>
       <c r="E68" s="10"/>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="3"/>
+      <c r="A69" s="4"/>
       <c r="B69" s="9"/>
       <c r="C69" s="10"/>
       <c r="D69" s="10"/>
       <c r="E69" s="10"/>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="3"/>
+      <c r="A70" s="4"/>
       <c r="B70" s="9"/>
       <c r="C70" s="10"/>
       <c r="D70" s="10"/>
       <c r="E70" s="10"/>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="3"/>
+      <c r="A71" s="4"/>
       <c r="B71" s="9"/>
       <c r="C71" s="10"/>
       <c r="D71" s="10"/>
       <c r="E71" s="10"/>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="4"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4221,30 +4241,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>